<commit_message>
Add bounding circles comparsion pdf.
</commit_message>
<xml_diff>
--- a/measurements/circle_performance_comparison.xlsx
+++ b/measurements/circle_performance_comparison.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aking\Documents\Alex\Work\CompSci\CS4098\brio-project\progression_images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aking\Documents\Alex\Work\CompSci\CS4098\brio-project\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC6FAA-1C0F-4BF1-ADED-B150F6D8C788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E95495-11B8-4566-87DE-0DD34F8F44FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{73B61109-674B-4C0C-A8E4-0DBF36CF5418}"/>
   </bookViews>
@@ -36,22 +36,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>with bounding circles</t>
+    <t>Seed</t>
   </si>
   <si>
-    <t>without circles</t>
+    <r>
+      <t>Completion time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (in ms, with out bounding circles)</t>
+    </r>
   </si>
   <si>
-    <t>seed</t>
+    <r>
+      <t xml:space="preserve">Completion time </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(in ms, with bounding circles)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Average completion time </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(in ms)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,13 +98,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +163,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,123 +489,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C08333-3019-4F09-81CA-E5086610BEF9}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="1" max="1" width="44.26953125" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" customWidth="1"/>
+    <col min="12" max="12" width="31.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="B1">
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3928</v>
+      </c>
+      <c r="C2" s="2">
+        <v>38536</v>
+      </c>
+      <c r="D2" s="2">
+        <v>32998</v>
+      </c>
+      <c r="E2" s="2">
+        <v>25983</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4232</v>
+      </c>
+      <c r="G2" s="2">
+        <v>35312</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5764</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7901</v>
+      </c>
+      <c r="J2" s="2">
+        <v>50573</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10011</v>
+      </c>
+      <c r="L2" s="6">
+        <f>AVERAGE(B2:K2)</f>
+        <v>21523.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>3928</v>
-      </c>
-      <c r="C2">
-        <v>38536</v>
-      </c>
-      <c r="D2">
-        <v>32998</v>
-      </c>
-      <c r="E2">
-        <v>25983</v>
-      </c>
-      <c r="F2">
-        <v>4232</v>
-      </c>
-      <c r="G2">
-        <v>35312</v>
-      </c>
-      <c r="H2">
-        <v>5764</v>
-      </c>
-      <c r="I2">
-        <v>7901</v>
-      </c>
-      <c r="J2">
-        <v>50573</v>
-      </c>
-      <c r="K2">
-        <v>10011</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>28253</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>250336</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>186734</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>177445</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>35221</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>235735</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>43350</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>52043</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>342449</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
         <v>85494</v>
+      </c>
+      <c r="L3" s="6">
+        <f>AVERAGE(B3:K3)</f>
+        <v>143706</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add description of the algorithm.
</commit_message>
<xml_diff>
--- a/measurements/circle_performance_comparison.xlsx
+++ b/measurements/circle_performance_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aking\Documents\Alex\Work\CompSci\CS4098\brio-project\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E95495-11B8-4566-87DE-0DD34F8F44FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB758C2-D791-4220-B6C5-1F8B2103D3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{73B61109-674B-4C0C-A8E4-0DBF36CF5418}"/>
   </bookViews>
@@ -190,6 +190,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{610E1862-118B-9F98-0C50-F120C9594E3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="171450" y="939800"/>
+          <a:ext cx="11417300" cy="558800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,7 +558,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,5 +687,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Present results in graphs.
</commit_message>
<xml_diff>
--- a/measurements/circle_performance_comparison.xlsx
+++ b/measurements/circle_performance_comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aking\Documents\Alex\Work\CompSci\CS4098\brio-project\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB758C2-D791-4220-B6C5-1F8B2103D3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74A64FD-4F72-492D-9CC9-B6533E95A935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{73B61109-674B-4C0C-A8E4-0DBF36CF5418}"/>
   </bookViews>
@@ -192,20 +192,1084 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> of track-generation time for set {100E, 30A, 100E1, 2L, 2M} for a range of seeds, with and without the inclusion of bounding circles.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>With bounding circles</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25983</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4232</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35312</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5764</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50573</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-736C-4BA5-AD9E-18A3B78E7446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Without bounding circles</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>28253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>186734</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>177445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>235735</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52043</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>342449</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85494</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-736C-4BA5-AD9E-18A3B78E7446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="624084664"/>
+        <c:axId val="624085016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="624084664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Seed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="624085016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="624085016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Generation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> time (in ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="624084664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -235,7 +1299,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="171450" y="939800"/>
+          <a:off x="107950" y="2387600"/>
           <a:ext cx="11417300" cy="558800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -253,6 +1317,42 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>357867</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1469572</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4B36D40-F4F1-056E-5C04-CAD4F23FF8F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -557,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C08333-3019-4F09-81CA-E5086610BEF9}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>